<commit_message>
Data leakage fixed; Edits in feature engineering
</commit_message>
<xml_diff>
--- a/Model performance log.xlsx
+++ b/Model performance log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23240" windowHeight="9316"/>
+    <workbookView windowWidth="29526" windowHeight="9754"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsblatt1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>KNN Regressor Performance Log</t>
   </si>
@@ -52,7 +52,97 @@
 Test R²: 0.622935612552125</t>
   </si>
   <si>
-    <t>k</t>
+    <t xml:space="preserve">Training MSE: 6173772612.184486
+Training R²: 0.8251709319010697
+Test MSE: 19927046689.381184
+Test R²: 0.4662687915386866
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 6144466819.101653
+Training R²: 0.8260008141815509
+Test MSE: 19770693602.73045
+Test R²: 0.47045659333318035
+</t>
+  </si>
+  <si>
+    <t>Training MSE: 2928012999.2489395
+Training R²: 0.9170844447639742
+Test MSE: 15447395075.405716
+Test R²: 0.5862529470777453</t>
+  </si>
+  <si>
+    <t>Training MSE: 244545669.77620947
+Training R²: 0.9930749487808759
+Test MSE: 10725945453.952984
+Test R²: 0.7127134834245609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 244565855.2060783
+Training R²: 0.9930743771692998
+Test MSE: 10903578231.508595
+Test R²: 0.7079557208466463
+Test MAE: 63564.31194670391
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 244565855.91001666
+Training R²: 0.9930743771493656
+Test MSE: 11369594519.724035
+Test R²: 0.695473819210694
+Test MAE: 64434.38539365518
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 244650205.07534486
+Training R²: 0.9930719885473073
+Test MSE: 11351818925.348797
+Test R²: 0.6959499253600347
+Test MAE: 64625.63924378763
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 244650203.60819906
+Training R²: 0.9930719885888539
+Test MSE: 10674049461.007736
+Test R²: 0.7141034792157448
+Test MAE: 63097.51904805294
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 271142436.92710483
+Training R²: 0.9923217807736417
+Test MSE: 10665601947.573637
+Test R²: 0.7143297396156905
+Test MAE: 63113.49606009365
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 244650203.60819906
+Training R²: 0.9930719885888539
+Test MSE: 10676699089.682962
+Test R²: 0.7140325108712207
+Test MAE: 63098.241992967785
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 363132288.1017958
+Training R²: 0.9897168095565791
+Test MSE: 11273026109.800705
+Test R²: 0.6980603326530012
+Test MAE: 65531.24314938047
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training MSE: 202167606.18209013
+Training R²: 0.994275011988804
+Test MSE: 11044787245.791832
+Test R²: 0.7041735418306666
+Test MAE: 64842.70390706739
+</t>
+  </si>
+  <si>
+    <t>best k</t>
   </si>
   <si>
     <t>weights</t>
@@ -64,7 +154,36 @@
     <t>features</t>
   </si>
   <si>
-    <t>living_area', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'swimming_pool', 'facade_number', 'garden'</t>
+    <t>living_area', 'latitude', 'longitude', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'swimming_pool', 'facade_number', 'garden'</t>
+  </si>
+  <si>
+    <t>location_cluster_sorted', 'living_area', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'swimming_pool', 'garden'</t>
+  </si>
+  <si>
+    <t>provinces_encoded', 'living_area', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'swimming_pool', 'garden'</t>
+  </si>
+  <si>
+    <t>communes_encoded', 'living_area', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'swimming_pool', 'garden'</t>
+  </si>
+  <si>
+    <t>['price', 'commune_encoded', 'living_area', 'garden', 'terrace',
+ 'swimming_pool', 'kitchen_installed', 'kitchen_not installed', 'kitchen_semi equipped', 'condition_good', 'condition_just renovated', 'condition_to be done up', 'condition_to renovate',    'condition_to restore', 'subtype_ house', 'subtype_luxury', 'subtype_ mixed use building', 'subtype_other']</t>
+  </si>
+  <si>
+    <t>['price', 'commune_encoded', 'living_area', 'garden', 'terrace',
+ 'kitchen_installed', 'kitchen_not installed', 'kitchen_semi equipped', 'condition_good', 'condition_just renovated', 'condition_to be done up', 'condition_to renovate',    'condition_to restore', 'subtype_ house', 'subtype_luxury', 'subtype_ mixed use building', 'subtype_other']</t>
+  </si>
+  <si>
+    <t>communes_encoded', 'living_area', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'garden'</t>
+  </si>
+  <si>
+    <t>communes_encoded', 'living_area', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace'</t>
+  </si>
+  <si>
+    <t>communes_encoded', 'living_area_building_condition', 'subtype_of_property', 'equipped_kitchen', 'terrace', 'garden'</t>
+  </si>
+  <si>
+    <t>communes_encoded', 'living_area_rooms', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'garden'</t>
   </si>
   <si>
     <t>log transformation</t>
@@ -83,6 +202,48 @@
   </si>
   <si>
     <t>removed in price</t>
+  </si>
+  <si>
+    <t>removed for price</t>
+  </si>
+  <si>
+    <t>Location Cluster</t>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>dummy encoding used for kitchen, subtype, and condition; binary data not standardized</t>
+  </si>
+  <si>
+    <t>dummy encoding used for kitchen, subtype, and condition; binary data standardized</t>
+  </si>
+  <si>
+    <t>dummy encoding used for kitchen, subtype, and condition; binary data standardized; swimming pool removed</t>
+  </si>
+  <si>
+    <t>label encoding for kitchen, subtype and condition; binary data standardized; swimming pool removed</t>
+  </si>
+  <si>
+    <t>label encoding for kitchen, subtype and condition; binary data standardized; swimming pool &amp; garden removed</t>
+  </si>
+  <si>
+    <t>Separation of training and test set BEFORE standardization; garden added back</t>
+  </si>
+  <si>
+    <t>Tried combination of living area and building condition</t>
+  </si>
+  <si>
+    <t>Tried combination of living area and number of rooms</t>
+  </si>
+  <si>
+    <t>Data leakage!</t>
+  </si>
+  <si>
+    <t>Leakage fixed</t>
   </si>
 </sst>
 </file>
@@ -95,7 +256,7 @@
     <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +266,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -255,12 +424,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -575,137 +762,137 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -713,6 +900,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
@@ -1251,19 +1468,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88495575221239" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88495575221239" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.1769911504425" customWidth="1"/>
-    <col min="2" max="2" width="29.141592920354" customWidth="1"/>
-    <col min="3" max="3" width="36.6725663716814" customWidth="1"/>
-    <col min="4" max="4" width="30.5752212389381" customWidth="1"/>
-    <col min="5" max="5" width="26.4778761061947" customWidth="1"/>
+    <col min="2" max="3" width="27.3716814159292" customWidth="1"/>
+    <col min="4" max="4" width="28.2477876106195" customWidth="1"/>
+    <col min="5" max="6" width="26.9203539823009" customWidth="1"/>
+    <col min="7" max="7" width="26.8053097345133" customWidth="1"/>
+    <col min="8" max="8" width="27.2566371681416" customWidth="1"/>
+    <col min="9" max="9" width="28.5840707964602" customWidth="1"/>
+    <col min="10" max="10" width="29.0265486725664" customWidth="1"/>
+    <col min="11" max="11" width="33.3451327433628" customWidth="1"/>
+    <col min="12" max="12" width="31.2389380530973" customWidth="1"/>
+    <col min="13" max="13" width="30.5752212389381" customWidth="1"/>
+    <col min="14" max="14" width="41.4424778761062" customWidth="1"/>
+    <col min="15" max="15" width="38" customWidth="1"/>
+    <col min="16" max="16" width="31.0176991150442" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.15" spans="1:1">
@@ -1271,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="75.15" spans="1:4">
+    <row r="3" ht="100" customHeight="1" spans="1:16">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1284,10 +1512,46 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>14</v>
@@ -1298,61 +1562,289 @@
       <c r="D4">
         <v>10</v>
       </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
+      </c>
+      <c r="L4" s="5">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>20</v>
+      </c>
+      <c r="O4">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="6" ht="75.15" spans="1:4">
+    <row r="6" ht="180.3" spans="1:16">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9">
         <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" ht="60.1" spans="1:16">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B13:M13"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Income imported; Result improved
</commit_message>
<xml_diff>
--- a/Model performance log.xlsx
+++ b/Model performance log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29526" windowHeight="9316"/>
+    <workbookView windowWidth="20998" windowHeight="9854"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsblatt1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>KNN Regressor Performance Log</t>
   </si>
@@ -142,6 +142,24 @@
 </t>
   </si>
   <si>
+    <t>Test Metrics:
+Mean Absolute Error (MAE): 64213.5778
+Root Mean Squared Error (RMSE): 93843.7746
+Mean Squared Error (MSE): 8808825644.0570
+R Squared: 0.5814
+Mean Absolute Percentage Error (MAPE): 20.3289
+Symmetric Mean Absolute Percentage Error (sMAPE): 18.2049</t>
+  </si>
+  <si>
+    <t>Test Metrics:
+Mean Absolute Error (MAE): 57784.1676
+Root Mean Squared Error (RMSE): 90250.1423
+Mean Squared Error (MSE): 8146874310.3034
+R Squared: 0.6129
+Mean Absolute Percentage Error (MAPE): 18.5094
+Symmetric Mean Absolute Percentage Error (sMAPE): 16.5011</t>
+  </si>
+  <si>
     <t>best k</t>
   </si>
   <si>
@@ -149,6 +167,9 @@
   </si>
   <si>
     <t>distance</t>
+  </si>
+  <si>
+    <t>uniform</t>
   </si>
   <si>
     <t>features</t>
@@ -186,6 +207,9 @@
     <t>communes_encoded', 'living_area_rooms', 'subtype_of_property', 'building_condition', 'equipped_kitchen', 'terrace', 'garden'</t>
   </si>
   <si>
+    <t>['commune_encoded', 'living_area', 'building_condition_encoded', 'terrace_encoded', 'equipped_kitchen_encoded', 'subtype_of_property_encoded', 'com_avg_income']</t>
+  </si>
+  <si>
     <t>log transformation</t>
   </si>
   <si>
@@ -207,12 +231,21 @@
     <t>removed for price</t>
   </si>
   <si>
+    <t xml:space="preserve">removed for price </t>
+  </si>
+  <si>
     <t>Location Cluster</t>
   </si>
   <si>
     <t>not used</t>
   </si>
   <si>
+    <t>Accuracy computing procedure</t>
+  </si>
+  <si>
+    <t>k-fold: 5</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -240,10 +273,10 @@
     <t>Tried combination of living area and number of rooms</t>
   </si>
   <si>
-    <t>Data leakage!</t>
-  </si>
-  <si>
-    <t>Leakage fixed</t>
+    <t>if I drop outliers in garden based on IQR, garden has only 0 values; metrics improve without 'garden' as feature</t>
+  </si>
+  <si>
+    <t>Data Leakage</t>
   </si>
 </sst>
 </file>
@@ -273,7 +306,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -424,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,12 +467,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,7 +789,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -786,16 +813,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -804,89 +831,89 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -905,11 +932,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1450,30 +1474,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="N3" sqref="N3"/>
+      <selection pane="topRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88495575221239" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.1769911504425" customWidth="1"/>
-    <col min="2" max="3" width="27.3716814159292" customWidth="1"/>
-    <col min="4" max="4" width="28.2477876106195" customWidth="1"/>
-    <col min="5" max="6" width="26.9203539823009" customWidth="1"/>
-    <col min="7" max="7" width="26.8053097345133" customWidth="1"/>
-    <col min="8" max="8" width="27.2566371681416" customWidth="1"/>
-    <col min="9" max="9" width="28.5840707964602" customWidth="1"/>
-    <col min="10" max="10" width="29.0265486725664" customWidth="1"/>
-    <col min="11" max="11" width="33.3451327433628" customWidth="1"/>
-    <col min="12" max="12" width="31.2389380530973" customWidth="1"/>
-    <col min="13" max="13" width="30.5752212389381" customWidth="1"/>
-    <col min="14" max="14" width="41.4424778761062" customWidth="1"/>
-    <col min="15" max="15" width="38" customWidth="1"/>
-    <col min="16" max="16" width="31.0176991150442" customWidth="1"/>
+    <col min="2" max="3" width="27.3716814159292" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="28.2477876106195" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="26.9203539823009" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="26.8053097345133" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.2566371681416" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5840707964602" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="29.0265486725664" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="33.3451327433628" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="31.2389380530973" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5752212389381" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="41.4424778761062" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="38" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="31.0176991150442" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="46.6814159292035" customWidth="1"/>
+    <col min="18" max="18" width="44.3274336283186" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.15" spans="1:1">
@@ -1481,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="100" customHeight="1" spans="1:16">
+    <row r="3" ht="165" customHeight="1" spans="1:18">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1521,7 +1547,7 @@
       <c r="M3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -1530,10 +1556,16 @@
       <c r="P3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="Q3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>14</v>
@@ -1577,175 +1609,205 @@
       <c r="O4">
         <v>28</v>
       </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H5" s="4"/>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6" ht="180.3" spans="1:16">
+    <row r="6" ht="180.3" spans="1:18">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="I6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="L6" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="M6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R7" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N8" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E9">
         <v>24</v>
@@ -1754,78 +1816,99 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>44</v>
+      </c>
+      <c r="R9" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="10" ht="60.1" spans="1:16">
+    <row r="10" ht="33" customHeight="1" spans="1:18">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="H10" s="4"/>
+      <c r="Q10" t="s">
         <v>46</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="R10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" ht="60.1" spans="1:17">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="7" t="s">
-        <v>50</v>
-      </c>
+    <row r="14" ht="23.75" spans="2:16">
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B14:P14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Function for sorted encoding implemented, but abandoned for commune
</commit_message>
<xml_diff>
--- a/Model performance log.xlsx
+++ b/Model performance log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
   <si>
     <t>KNN Regressor Performance Log</t>
   </si>
@@ -196,6 +196,15 @@
 Symmetric Mean Absolute Percentage Error (sMAPE): 22.9009</t>
   </si>
   <si>
+    <t>Test Metrics:
+Mean Absolute Error (MAE): 60057.7877
+Root Mean Squared Error (RMSE): 93245.4747
+Mean Squared Error (MSE): 8697058022.8145
+R Squared: 0.5869
+Mean Absolute Percentage Error (MAPE): 19.1404
+Symmetric Mean Absolute Percentage Error (sMAPE): 17.1467</t>
+  </si>
+  <si>
     <t>best k</t>
   </si>
   <si>
@@ -256,6 +265,9 @@
   </si>
   <si>
     <t>living_area', 'building_condition_encoded', 'terrace_encoded', 'equipped_kitchen_encoded', 'subtype_of_property_encoded', 'commune_income_cluster'</t>
+  </si>
+  <si>
+    <t>['commune_encoded_sorted', 'living_area', 'building_condition_encoded', 'terrace_encoded', 'equipped_kitchen_encoded', 'subtype_of_property_encoded', 'com_avg_income', 'commune_income_cluster']</t>
   </si>
   <si>
     <t>log transformation</t>
@@ -523,7 +535,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,6 +545,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,7 +873,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -879,16 +897,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -897,85 +915,85 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -989,9 +1007,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1001,13 +1016,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1546,9 +1561,9 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="W6" sqref="W6"/>
+      <selection pane="topRight" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88495575221239" defaultRowHeight="15"/>
@@ -1573,7 +1588,7 @@
     <col min="20" max="20" width="39.7345132743363" customWidth="1"/>
     <col min="21" max="21" width="41.8053097345133" customWidth="1"/>
     <col min="22" max="22" width="44.7610619469027" customWidth="1"/>
-    <col min="23" max="23" width="34.212389380531" customWidth="1"/>
+    <col min="23" max="23" width="39.3982300884956" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.15" spans="1:1">
@@ -1581,62 +1596,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="135.25" spans="1:22">
+    <row r="3" s="1" customFormat="1" ht="135.25" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="T3" s="1" t="s">
@@ -1647,11 +1662,14 @@
       </c>
       <c r="V3" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>14</v>
@@ -1671,7 +1689,7 @@
       <c r="G4">
         <v>29</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>17</v>
       </c>
       <c r="I4">
@@ -1683,7 +1701,7 @@
       <c r="K4">
         <v>20</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>20</v>
       </c>
       <c r="M4">
@@ -1710,232 +1728,241 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="H5" s="4"/>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="Q5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
         <v>26</v>
       </c>
-      <c r="R5" t="s">
-        <v>25</v>
-      </c>
       <c r="S5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="180.3" spans="1:22">
+    <row r="6" s="1" customFormat="1" ht="180.3" spans="1:23">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="I6" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="L6" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="O6" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" s="9" t="s">
+      <c r="Q6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="R6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="T6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="U6" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="V6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="S7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="U7" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="W7" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Q8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="S8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U8" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="W8" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E9">
         <v>24</v>
@@ -1944,125 +1971,131 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="R9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="U9" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="W9" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="10" ht="33" customHeight="1" spans="1:21">
+    <row r="10" ht="33" customHeight="1" spans="1:23">
       <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="H10" s="4"/>
       <c r="Q10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="S10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="T10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="U10" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="W10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="60.1" spans="1:23">
       <c r="A11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="I11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="J11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="K11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="L11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="M11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="N11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="O11" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="P11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="T11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="U11" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" ht="23.75" spans="2:16">
-      <c r="B14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="B14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>